<commit_message>
Added one variable, two variable, and multiple equations
</commit_message>
<xml_diff>
--- a/MATT/bin/Debug/MATT_Instructions.xlsx
+++ b/MATT/bin/Debug/MATT_Instructions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>SciNotation</t>
   </si>
@@ -273,6 +273,131 @@
   <si>
     <t xml:space="preserve">When a variable with a coefficient is raised to a power, the power is "distributed" to the coefficient and the variable.
 &lt;\MATTPics\CoefVarToPower_Example.png&gt;
+</t>
+  </si>
+  <si>
+    <t>PullOutAnX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When two terms have a term in common, it can be factored out of the terms in order to simplify the expression. This is the opposite of distrubuting a term.
+&lt;\MATTPics\PullOutAnX_Example.png&gt;
+</t>
+  </si>
+  <si>
+    <t>To get a variable by itself when it is being divided by a constant, multiply both sides of the equation by the constant.
+&lt;\MATTPics\RemoveDenomConst_Mult.png&gt;
+You can also think of the constant as a fractional coefficient and then divide both sides of the equation by the fraction. This will get you the same result as the above process, but is just a different way to think about it.
+&lt;\MATTPics\RemoveDenomConst_DivFrac.png&gt;</t>
+  </si>
+  <si>
+    <t>RemoveDenomConst</t>
+  </si>
+  <si>
+    <t>CircleEqn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The equation of a circle looks like the one below. The right hand side of the equation will tell you the radius of the circle. The center of the circle is the value being subtracted from each value. If there is no value being subtracted then the center point is (0,0).
+&lt;\MATTPics\CircleEqn_Formula.png&gt;
+</t>
+  </si>
+  <si>
+    <t>GraphYEq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When an equation is in the form "y = mx + b", m is the value for the slope and b is the y-intercept. The slope represents the change in the y values divided by the change in the x values. The y-intercept is the value of x when y is 0.
+&lt;\MATTPics\GraphYEq_Formula.png&gt;
+</t>
+  </si>
+  <si>
+    <t>SolveForY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To put an equation in y=mx+b form, you want to get the y by itself. Move all of the other terms to the right-hand side of the equals sign.
+&lt;\MATTPics\SolveForY_MoveTerms.png&gt;
+If there is a coefficient in front of the y term, divide the equation by the coefficient. Make sure you divide every term on the right-hand side.
+&lt;\MATTPics\SolveForY_Coef.png&gt;
+</t>
+  </si>
+  <si>
+    <t>EllipseEqn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The equation of an ellipse is similar to that of a circle except that an ellipse equation has fractional values. The denominators of these fractions represent the length of the major axis and minor axis of the ellipse. The center and radius are the same as for the equation of a circle.
+&lt;\MATTPics\EllipseEqn_Example.png&gt;
+</t>
+  </si>
+  <si>
+    <t>VParabola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An equation with the degree of y = 1 and the degree of x = 2 will graph to be a vertical parabola. The most basic parabola is y = x^2.
+&lt;\MATTPics\VParabola_Basic.png&gt;
+A more complex equation for a parabola could be moved off the origin and be made skinnier or fatter. The general formula for a parabola is below. The coefficient, a, tells you whether the parabola opens up or down and how skinny or fat the parabola is. The variables h and k tell you the vertex of the parabola.
+&lt;\MATTPics\VParabola_Formula.png&gt;
+</t>
+  </si>
+  <si>
+    <t>HParabola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An equation that can be set up as "x=" with the degree of y = 2 is a horizontal parabola. These parabolas open to the left or right rather than up or down. For a "sideways" parabola, if the value of a is negative, it will open to the left and ir a is positive it will open to the right. The other variables in the equation are the same as for a vertical parabola.
+&lt;\MATTPics\HParabola_Example.png&gt;
+</t>
+  </si>
+  <si>
+    <t>Intercepts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An intercept is the point where the line crosses the x or y axis. The x-intercepts is the point where the line crosses the x-axis and the y-intercept is the point where the line crosses the y-axis. Equations whose degree is greater than 1 could have more than one intercept on one axis and/or no intercept on the other axis. For example, a parabola could never cross the x-axis if the vertex is above the axis or it could cross in two places if the vertex is below the axis. The below example has 3 x-intercepts and 1 y-intercept.
+&lt;\MATTPics\Intercepts_Example.png&gt;
+To find the x intercept of an equation, plug x=0 into the equaion and solve for y. The resulting y value gives you the point (0, y) which is your x intercept. Do the same process to find the y intercept but plug in y=0 to get a point of the form (x, 0).
+&lt;\MATTPics\Intercepts_MathExample.png&gt;
+</t>
+  </si>
+  <si>
+    <t>StandardForm</t>
+  </si>
+  <si>
+    <t>GraphLinear</t>
+  </si>
+  <si>
+    <t>GraphNonLinear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The standard form of a linear equation is Ax + By = C. To put an equation in standard form, the x and y need to both be on the right-hand side of the equation. The A coefficient needs to be positive. Heres an example:
+&lt;\MATTPics\StandardForm_Example.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The easiest way to graph and equation is to put the equation into slope-intercept form, aka y=mx+b form. The slope-intercept form makes it easy to see what the slope of the equation and its y-intercept. We can use these two pieces of information to easily graph the line.
+&lt;\MATTPics\GraphLinear_SlopeIntercept.png&gt;
+If the equation is not in slope-intercept form, you can always find the slope using two points of the line. Once you know the slope, you can pick any starting point that is on the line (hint: use one of the points you used to find the slope). Mark points along the line by moving in the y direction the number of points in the numerator of the slope and moving in the x direction the number of points in the denominator of the slope.
+&lt;\MATTPics\GraphLinear_PointSlope.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Graphing non-linear equations is easy if you already know what general shape the equation represents. Shapes whose equations you should be able to recognize are circles, ellipses, parabolas, and hyperbolas. If you do not know what shape the equation is representing, you can always create a table of x and y values and connect the points in the table.
+&lt;\MATTPics\GraphNonLinear_Shapes.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hyperbolas look like two parabolas in one graph. They're equation looks very similar to the equation for an ellipse but the terms are being subtracted instead of added. Because of this subtraction, the order of the terms is important.
+&lt;\MATTPics\Hyperbola_Formula.png&gt;
+The vertices of the "parabolas" are a or b distance from the center point. The branches of the hyperbola are bounded by asymptotes. The fundamental rectangle (a by b) will help you graph the asymptotes and the hyperbola.
+&lt;\MATTPics\Hyperbola_GraphAsym.png&gt;
+</t>
+  </si>
+  <si>
+    <t>Hyperbola</t>
+  </si>
+  <si>
+    <t>MultEqn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are several ways to solve systems of equations.To be able to solve a system of equations you need as many equation as unknown variables. For linear equations, the solution to the system is the point of intersection of the two lines. Keep in mind that if the lines don't actually intersect then you won't get a logical answer when trying to solve the system. One way is to use substitution. Using substitution to solve a system of equations means that you solve one of the equations for a variable and then plug-in that value into another equation. Once you have equations for all the variables, you plug in the values you found until you have a value for all of the variables.
+&lt;\MATTPics\MultEqn_Substitution.png&gt;
+Another way to solve a system of equations is to use matrices. For this method, you create a matrix of coefficients and solutions and then use row operations to reduce the coefficients to the identity matrix.
+&lt;\MATTPics\MultEqn_Matrix.png&gt;
 </t>
   </si>
 </sst>
@@ -597,10 +722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B24"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -801,6 +926,118 @@
         <v>47</v>
       </c>
     </row>
+    <row r="25" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added basic trigonometry problems
</commit_message>
<xml_diff>
--- a/MATT/bin/Debug/MATT_Instructions.xlsx
+++ b/MATT/bin/Debug/MATT_Instructions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
   <si>
     <t>SciNotation</t>
   </si>
@@ -400,18 +400,78 @@
 &lt;\MATTPics\MultEqn_Matrix.png&gt;
 </t>
   </si>
+  <si>
+    <t>TriangleTrig</t>
+  </si>
+  <si>
+    <t>UnitCircle</t>
+  </si>
+  <si>
+    <t>RadToDeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Unit Circle is a circle of radius 1 centered at the origin. The degrees around the circle are usually presented in radians but it is important to know which degrees correspond to the radian value.
+&lt;\MATTPics\UnitCircle_Angles.png&gt;
+The points on the circle are listed as (cosinse, sine) rather than (x, y). There are three values that are seen in the points between the axises: 1/2, √2/2, and √3/2. These points are used to know the values of sine and cosine for th angles in radians.
+&lt;\MATTPics\UnitCircle_Points.png&gt;
+Here is the whole enchilada in radians and degrees with an example:
+&lt;\MATTPics\UnitCircle_Complete.png&gt;
+&lt;\MATTPics\UnitCircle_Example.png&gt;
+</t>
+  </si>
+  <si>
+    <r>
+      <t>Degrees are a representation of revolution around a point. If you start at 0 degress and turn completely, stopping where you started, then you rotated 360 degrees. In that way, degrees are like percentages, and you have to convert percentages to decimals before doing math with them. There is a similar relationship between degrees and radians. Radians represent the fraction of the Unit Circle that the revolution corresponds to.
+&lt;\MATTPics\RadToDeg_Equations.png&gt;
+ The conversion between the two values is based on the fact that a full revolution in degrees is 360 degrees and a full revolution in radians in 2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">π.
+&lt;\MATTPics\RadToDeg_Example.png&gt;
+</t>
+    </r>
+  </si>
+  <si>
+    <t>TrigProps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The properites and identites of the trigonometric functions are important to know because they are often used to simplify problems.
+&lt;\MATTPics\TrigProps.png&gt; 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An easy way to remember how the trigonometric function sine, cosine, and tangent work is to use the acronym soh cah toa.
+&lt;\MATTPics\TriangleTrig_SohCahToa.png&gt;
+This method can be used to calculate the sine, cosine, or tangent of a given angle within a right triangle. An example is below.
+&lt;\MATTPics\TriangleTrig_Example.png&gt;
+A typical question, however, will not give you all of the information but will ask you to use the trigonometric function to solve for one of the values of the triangle. Here are the definitions of all of the trigonometric functions.
+&lt;\MATTPics\TriangleTrig_Functions.png&gt;
+</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -722,10 +782,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1038,7 +1098,40 @@
         <v>75</v>
       </c>
     </row>
+    <row r="39" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="216" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A42" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added Basics for Trigonmetry and Logarithms
</commit_message>
<xml_diff>
--- a/MATT/bin/Debug/MATT_Instructions.xlsx
+++ b/MATT/bin/Debug/MATT_Instructions.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="126">
   <si>
     <t>SciNotation</t>
   </si>
@@ -51,16 +51,6 @@
     <t>OrderOfOperations</t>
   </si>
   <si>
-    <t xml:space="preserve">Order of Operations (PEDMAS)
-There is a heirarchy of operations when evaluating matematical expressions:
-1. Parentheses: Always evaluate expressions inside parentheses first.
-2. Exponents: Next apply any exponents in the expression (This step also applies to radicals).
-3/4. Division/Mutiplication: Since division and multiplication are the same step, evaluate from right to left.
-5/6. Addition/Subtraction: Also evaluate additon and subraction from right to left.
-A way to help remember this order is to use the neumonic device Please Excuse My Dear Aunt Sally.
-</t>
-  </si>
-  <si>
     <t>FractionExponent</t>
   </si>
   <si>
@@ -115,17 +105,6 @@
     <t>RadicalsEqn</t>
   </si>
   <si>
-    <t xml:space="preserve">A number with an exponent written above it is a shorter way to write how many times a number is multiplied by itself.
-The larger number is the base and the smaller number written above it is the exponent.
-&lt;\MATTPics\SimpleExponent_BaseExp.png&gt;
-The base is multiplied by itself the number of times that the exponent indicates:
-&lt;\MATTPics\SimpleExponent_Expanded.png&gt;
-This is also called rasing a number to a power.
-A negative exponent will be positive in the denominator of an expression. Once the exponent is positive, it can be evaluated normally.
-&lt;\MATTPics\SimpleExponent_Negative.png&gt;
-</t>
-  </si>
-  <si>
     <t>FOIL</t>
   </si>
   <si>
@@ -198,28 +177,6 @@
   <si>
     <t xml:space="preserve">Distribute the single term into the parenthesis. Then simplify the expression.
 &lt;\MATTPics\Distribution_Example.PNG&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Multiplying two polynomials involves multiplying each term in both of the polynomials. Remeber that when an entire equation is raised to a power, you can't simply distribute the power, you have to multiply the equations together. This process is commonly referred to as FOIL. FOIL stands for
-First
-Outside
-Inside
-Last
-It represents the order of multiplying each term in the two equations. Here are a couple examples:
-&lt;\MATTPics\FOIL_BreakDown.png&gt;
-&lt;\MATTPics\FOIL_Example.png&gt;
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If you can factor out of the numerator a term than can also be factored out of the denomenator, then these terms will cancel. Be careful that the term you pull out is common to all of the terms in the numerator and denominator.
-&lt;\MATTPics\CancelDivision_Example2.PNG&gt;
-You can also apply this technique to variable denominators.
-&lt;\MATTPics\CancelDivision_Example.PNG&gt;
-If you cannot factor out any common terms, you can separate the fraction into several terms. This can only be done if the numerator is multiple terms.
-&lt;\MATTPics\CancelDivision_Separate.PNG&gt;
-If the numerator is only one term, the fraction can still be separated but only by a process called partial fraction decomposition.
-&lt;\MATTPics\PartialFractions.PNG&gt;
 </t>
   </si>
   <si>
@@ -239,19 +196,7 @@
     <t>MultDivNumVar</t>
   </si>
   <si>
-    <t xml:space="preserve">When a variable term is multiplied or diveded by a constant, the operation is applied to the coefficient.
-&lt;\MATTPics\MultDivNumVar_Example.png&gt;
-Be careful because if x is in the denominator then it carries a negative exponent!
-&lt;\MATTPics\MultDivNumVar_NegExp.png&gt;
-</t>
-  </si>
-  <si>
     <t>Rationalize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">To rationalize an expression, get the radical out of the denominator, you have to muliply the fraction by the conjugate of the radical. The conjugate is a quantity that cancels out the radical in an expression. It always has the same expression under the radical you are trying to get rid of except with the opposite operation.
-&lt;\MATTPics\Rationalize_Example.png&gt;
-</t>
   </si>
   <si>
     <t xml:space="preserve">To remove a radical from one side of an equation, raise both sides of the equation to the reciprocal of the radical value. Make sure that you first get the radical by itself, or else you have to square each term in the equation.
@@ -277,11 +222,6 @@
   </si>
   <si>
     <t>PullOutAnX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">When two terms have a term in common, it can be factored out of the terms in order to simplify the expression. This is the opposite of distrubuting a term.
-&lt;\MATTPics\PullOutAnX_Example.png&gt;
-</t>
   </si>
   <si>
     <t>To get a variable by itself when it is being divided by a constant, multiply both sides of the equation by the constant.
@@ -340,21 +280,9 @@
     <t>HParabola</t>
   </si>
   <si>
-    <t xml:space="preserve">An equation that can be set up as "x=" with the degree of y = 2 is a horizontal parabola. These parabolas open to the left or right rather than up or down. For a "sideways" parabola, if the value of a is negative, it will open to the left and ir a is positive it will open to the right. The other variables in the equation are the same as for a vertical parabola.
-&lt;\MATTPics\HParabola_Example.png&gt;
-</t>
-  </si>
-  <si>
     <t>Intercepts</t>
   </si>
   <si>
-    <t xml:space="preserve">An intercept is the point where the line crosses the x or y axis. The x-intercepts is the point where the line crosses the x-axis and the y-intercept is the point where the line crosses the y-axis. Equations whose degree is greater than 1 could have more than one intercept on one axis and/or no intercept on the other axis. For example, a parabola could never cross the x-axis if the vertex is above the axis or it could cross in two places if the vertex is below the axis. The below example has 3 x-intercepts and 1 y-intercept.
-&lt;\MATTPics\Intercepts_Example.png&gt;
-To find the x intercept of an equation, plug x=0 into the equaion and solve for y. The resulting y value gives you the point (0, y) which is your x intercept. Do the same process to find the y intercept but plug in y=0 to get a point of the form (x, 0).
-&lt;\MATTPics\Intercepts_MathExample.png&gt;
-</t>
-  </si>
-  <si>
     <t>StandardForm</t>
   </si>
   <si>
@@ -362,11 +290,6 @@
   </si>
   <si>
     <t>GraphNonLinear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The standard form of a linear equation is Ax + By = C. To put an equation in standard form, the x and y need to both be on the right-hand side of the equation. The A coefficient needs to be positive. Heres an example:
-&lt;\MATTPics\StandardForm_Example.png&gt;
-</t>
   </si>
   <si>
     <t xml:space="preserve">The easiest way to graph and equation is to put the equation into slope-intercept form, aka y=mx+b form. The slope-intercept form makes it easy to see what the slope of the equation and its y-intercept. We can use these two pieces of information to easily graph the line.
@@ -394,13 +317,6 @@
     <t>MultEqn</t>
   </si>
   <si>
-    <t xml:space="preserve">There are several ways to solve systems of equations.To be able to solve a system of equations you need as many equation as unknown variables. For linear equations, the solution to the system is the point of intersection of the two lines. Keep in mind that if the lines don't actually intersect then you won't get a logical answer when trying to solve the system. One way is to use substitution. Using substitution to solve a system of equations means that you solve one of the equations for a variable and then plug-in that value into another equation. Once you have equations for all the variables, you plug in the values you found until you have a value for all of the variables.
-&lt;\MATTPics\MultEqn_Substitution.png&gt;
-Another way to solve a system of equations is to use matrices. For this method, you create a matrix of coefficients and solutions and then use row operations to reduce the coefficients to the identity matrix.
-&lt;\MATTPics\MultEqn_Matrix.png&gt;
-</t>
-  </si>
-  <si>
     <t>TriangleTrig</t>
   </si>
   <si>
@@ -410,18 +326,234 @@
     <t>RadToDeg</t>
   </si>
   <si>
-    <t xml:space="preserve">The Unit Circle is a circle of radius 1 centered at the origin. The degrees around the circle are usually presented in radians but it is important to know which degrees correspond to the radian value.
-&lt;\MATTPics\UnitCircle_Angles.png&gt;
-The points on the circle are listed as (cosinse, sine) rather than (x, y). There are three values that are seen in the points between the axises: 1/2, √2/2, and √3/2. These points are used to know the values of sine and cosine for th angles in radians.
-&lt;\MATTPics\UnitCircle_Points.png&gt;
-Here is the whole enchilada in radians and degrees with an example:
-&lt;\MATTPics\UnitCircle_Complete.png&gt;
-&lt;\MATTPics\UnitCircle_Example.png&gt;
+    <t>TrigProps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An easy way to remember how the trigonometric function sine, cosine, and tangent work is to use the acronym soh cah toa.
+&lt;\MATTPics\TriangleTrig_SohCahToa.png&gt;
+This method can be used to calculate the sine, cosine, or tangent of a given angle within a right triangle. An example is below.
+&lt;\MATTPics\TriangleTrig_Example.png&gt;
+A typical question, however, will not give you all of the information but will ask you to use the trigonometric function to solve for one of the values of the triangle. Here are the definitions of all of the trigonometric functions.
+&lt;\MATTPics\TriangleTrig_Functions.png&gt;
+</t>
+  </si>
+  <si>
+    <t>TrigReciprocalIDs</t>
+  </si>
+  <si>
+    <t>TrigDoubleAngle</t>
+  </si>
+  <si>
+    <t>TrigProductSum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Product to Sum properties of the trigonometry functions can be used if the sine and/or cosine functions are being multiplied and have different variables.
+&lt;\MATTPics\TrigProductSum.png&gt;
+</t>
+  </si>
+  <si>
+    <t>TrigSumProduct</t>
+  </si>
+  <si>
+    <t>TrigSumDiff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Sum and Difference formulas allow the expansion or contraction of the below situations.
+&lt;\MATTPics\TrigSumDiff.png&gt;
+</t>
+  </si>
+  <si>
+    <t>TrigHalfAngle</t>
+  </si>
+  <si>
+    <t>TrigEvenOdd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All of the trigonometry functions are either even or odd. To be an odd function means that a negative can be pulled from inside the function out to the front of the function. Even functions are always positive even if you get rid of the negative inside the parenthesis.
+&lt;\MATTPics\TrigEvenOdd.png&gt;
+</t>
+  </si>
+  <si>
+    <t>TrigPy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sum to product identities show how to write the product of trigonometric functions as a sum.
+&lt;\MATTPics\TrigSumProduct.png&gt;
 </t>
   </si>
   <si>
     <r>
-      <t>Degrees are a representation of revolution around a point. If you start at 0 degress and turn completely, stopping where you started, then you rotated 360 degrees. In that way, degrees are like percentages, and you have to convert percentages to decimals before doing math with them. There is a similar relationship between degrees and radians. Radians represent the fraction of the Unit Circle that the revolution corresponds to.
+      <t xml:space="preserve">The Half Angle formulas can be represented in two different ways. These formulas are handy if you are trying to find the value of a trigonometric function at an uncommon angle. For example, you could evaluate sin(120) by using the half angle formula and the fact that sin(60) = </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>√3/2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+&lt;\MATTPics\TrigHalfAngle.png&gt;
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The sine, cosine, and tangent functions can be expanded if they are called on two times the angle. These formulas can be useful for finding the value of a trigonometric function at an uncommon angle. For example, you could evaluate sin(15) using the fact that sin(30) = 1/2.
+&lt;\MATTPics\TrigDoubleAngle.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trigonometric functions can be simplified or expanded based on their definitions and reciprocal identites.
+&lt;\MATTPics\TrigReciprocalIDs.png&gt;
+</t>
+  </si>
+  <si>
+    <t>LogBasics</t>
+  </si>
+  <si>
+    <t>LnBasics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The natural logarithm is a logarithm with base of the mathematical constant e. It is written as ln() rather than with a subscript of e. Other than this notation, the natural log functions the same way as any other logarithm.
+</t>
+  </si>
+  <si>
+    <t>LogLaws</t>
+  </si>
+  <si>
+    <t>LogDivision</t>
+  </si>
+  <si>
+    <t>LogMultiplication</t>
+  </si>
+  <si>
+    <t>LogExponent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A logarithm that contains the product of two numbers can be separated into the sum of two logarithms.
+&lt;\MATTPics\LogMultiplication.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A logarithm that contains a value being raised to a power can be simplified by making the exponent a coefficient of the logarithm. This is derived from fact that a number raised to a power is the same as that number being multiplied by itself several times.
+&lt;\MATTPics\LogExponent.png&gt;
+</t>
+  </si>
+  <si>
+    <t>LogChangeBase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The base of a logarithm can be changed by dividing the logarithm by the log of the desired base.
+&lt;\MATTPics\LogChangeBase.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If the logarithm of a quotient can be separated into the difference of two logarithms.
+&lt;\MATTPics\LogDivision.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logarithms represent the relationship between bases and exponents. Logarithms can have any number as a base, but the most common are 10, e, and 2. When a logarithm has the base of 10, the subscript is commonly not written. Similarly, when a logarithm is base e, it is written as ln, the natural log. Here is the definition of a logarithm:
+&lt;\MATTPics\LogBasics_Defn.png&gt;
+</t>
+  </si>
+  <si>
+    <t>BasicAddSub</t>
+  </si>
+  <si>
+    <t>AddSubFrac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To solve this problem, you need to add or subtract the quantities. Addition is bringing two numbers together to make one total.
+&lt;\MATTPics\BasicAddSub_Add.png&gt;
+Subtraction is taking one number away from another.
+&lt;\MATTPics\BasicAddSub_Sub.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adding and subtracting fractions is a little different than adding or subtraction regular numbers. There are three steps to adding or subtracting fractions.
+Step 1: Make sure the bottom numbers (the denominators) match.
+Step 2: Add/Subtract the top numbers (the numerators) and put the answer over the denominator.
+Step 3: Simplify the fraction (if needed)
+Here is an example:
+&lt;\MATTPics\AddSubFrac_Example.png&gt;
+</t>
+  </si>
+  <si>
+    <t>BasicMult</t>
+  </si>
+  <si>
+    <t>MultFrac</t>
+  </si>
+  <si>
+    <t>BasicDiv</t>
+  </si>
+  <si>
+    <t>DivFrac</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiplying two, single-digit numbers is the easiest multiplications problem. However, it requires memorizing factors and products.
+&lt;\MATTPics\BasicMult_SingleDigit.png&gt;
+Multiplying becomes more difficult when the numbers are larger. You can make it easier by breaking the problem into smaller products.
+&lt;\MATTPics\BasicMult_Larger.png&gt;
+There is also a shorter way to perform this multiplication.
+&lt;\MATTPics\BasicMult_Shorthand.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiplying fractions is easier than it sounds. It only takes three steps:
+Step 1: Multiply the top numbers (numerators)
+Step 2: Multiply the bottom numbers (denominators)
+Step 3: Simplify the fraction, if needed
+Here is a simple example:
+&lt;\MATTPics\MultFrac_Example.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To divide two fractions, you simple flip the bottom fraction and then multiply them. You can remember this using the rhyme: "When dividing fractions, don't be shy. Just flip the second and multiply."
+&lt;\MATTPics\DivFrac_Example.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Two numbers are divided to find out how many times a number is contained in another number. Finding a quotient is the opposite of multiplying two numbers. You will need to ask yourself what product of quotient and divisor create a number closest to the dividend.
+&lt;\MATTPics\BasicDiv_Terms.png&gt;
+Long division is used for larger dividends when the answer is not so obvious. It takes several steps where you find a quotient for pieces of the larger proble. Study this example:
+&lt;\MATTPics\BasicDiv_LongDivision.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are a few simple properties of logarithms that might come in handy:
+&lt;\MATTPics\LogBasics_Zero.png&gt;
+&lt;\MATTPics\LogBasics_One.png&gt;
+&lt;\MATTPics\LogBasics_X.png&gt;
+There are also three properties of logarithms that can be helpful in simplifying expressions with logarithms:
+&lt;\MATTPics\LogLaws_All.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Pythagorean identities are derived from the Pythagorean theorem applied to the triangles made by the unit circle whose legs are the sine and cosine functions.
+&lt;\MATTPics\TrigPy.png&gt;
+&lt;\MATTPics\TrigPy_Circle.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The properties and identities of the trigonometric functions are important to know because they are often used to simplify problems.
+&lt;\MATTPics\TrigProps.png&gt; 
+</t>
+  </si>
+  <si>
+    <r>
+      <t>Degrees are a representation of revolution around a point. If you start at 0 degrees and turn completely, stopping where you started, then you rotated 360 degrees. In that way, degrees are like percentages, and you have to convert percentages to decimals before doing math with them. There is a similar relationship between degrees and radians. Radians represent the fraction of the Unit Circle that the revolution corresponds to.
 &lt;\MATTPics\RadToDeg_Equations.png&gt;
  The conversion between the two values is based on the fact that a full revolution in degrees is 360 degrees and a full revolution in radians in 2</t>
     </r>
@@ -438,20 +570,97 @@
     </r>
   </si>
   <si>
-    <t>TrigProps</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The properites and identites of the trigonometric functions are important to know because they are often used to simplify problems.
-&lt;\MATTPics\TrigProps.png&gt; 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An easy way to remember how the trigonometric function sine, cosine, and tangent work is to use the acronym soh cah toa.
-&lt;\MATTPics\TriangleTrig_SohCahToa.png&gt;
-This method can be used to calculate the sine, cosine, or tangent of a given angle within a right triangle. An example is below.
-&lt;\MATTPics\TriangleTrig_Example.png&gt;
-A typical question, however, will not give you all of the information but will ask you to use the trigonometric function to solve for one of the values of the triangle. Here are the definitions of all of the trigonometric functions.
-&lt;\MATTPics\TriangleTrig_Functions.png&gt;
+    <t xml:space="preserve">The Unit Circle is a circle of radius 1 centered at the origin. The degrees around the circle are usually presented in radians but it is important to know which degrees correspond to the radian value.
+&lt;\MATTPics\UnitCircle_Angles.png&gt;
+The points on the circle are listed as (cosine, sine) rather than (x, y). There are three values that are seen in the points between the axes: 1/2, √2/2, and √3/2. These points are used to know the values of sine and cosine for the angles in radians.
+&lt;\MATTPics\UnitCircle_Points.png&gt;
+Here is the whole enchilada in radians and degrees with an example:
+&lt;\MATTPics\UnitCircle_Complete.png&gt;
+&lt;\MATTPics\UnitCircle_Example.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are several ways to solve systems of equations. To be able to solve a system of equations you need as many equation as unknown variables. For linear equations, the solution to the system is the point of intersection of the two lines. Keep in mind that if the lines don't actually intersect then you won't get a logical answer when trying to solve the system. One way is to use substitution. Using substitution to solve a system of equations means that you solve one of the equations for a variable and then plug-in that value into another equation. Once you have equations for all the variables, you plug in the values you found until you have a value for all of the variables.
+&lt;\MATTPics\MultEqn_Substitution.png&gt;
+Another way to solve a system of equations is to use matrices. For this method, you create a matrix of coefficients and solutions and then use row operations to reduce the coefficients to the identity matrix.
+&lt;\MATTPics\MultEqn_Matrix.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The standard form of a linear equation is Ax + By = C. To put an equation in standard form, the x and y need to both be on the right-hand side of the equation. The A coefficient needs to be positive. Here's an example:
+&lt;\MATTPics\StandardForm_Example.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An intercept is the point where the line crosses the x or y axis. The x-intercepts is the point where the line crosses the x-axis and the y-intercept is the point where the line crosses the y-axis. Equations whose degree is greater than 1 could have more than one intercept on one axis and/or no intercept on the other axis. For example, a parabola could never cross the x-axis if the vertex is above the axis or it could cross in two places if the vertex is below the axis. The below example has 3 x-intercepts and 1 y-intercept.
+&lt;\MATTPics\Intercepts_Example.png&gt;
+To find the x intercept of an equation, plug x=0 into the equation and solve for y. The resulting y value gives you the point (0, y) which is your x intercept. Do the same process to find the y intercept but plug in y=0 to get a point of the form (x, 0).
+&lt;\MATTPics\Intercepts_MathExample.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An equation that can be set up as "x=" with the degree of y = 2 is a horizontal parabola. These parabolas open to the left or right rather than up or down. For a "sideways" parabola, if the value of a is negative, it will open to the left and if a is positive it will open to the right. The other variables in the equation are the same as for a vertical parabola.
+&lt;\MATTPics\HParabola_Example.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When two terms have a term in common, it can be factored out of the terms in order to simplify the expression. This is the opposite of distributing a term.
+&lt;\MATTPics\PullOutAnX_Example.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">To rationalize an expression, get the radical out of the denominator, you have to multiply the fraction by the conjugate of the radical. The conjugate is a quantity that cancels out the radical in an expression. It always has the same expression under the radical you are trying to get rid of except with the opposite operation.
+&lt;\MATTPics\Rationalize_Example.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When a variable term is multiplied or divided by a constant, the operation is applied to the coefficient.
+&lt;\MATTPics\MultDivNumVar_Example.png&gt;
+Be careful because if x is in the denominator then it carries a negative exponent!
+&lt;\MATTPics\MultDivNumVar_NegExp.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you can factor out of the numerator a term than can also be factored out of the denominator, then these terms will cancel. Be careful that the term you pull out is common to all of the terms in the numerator and denominator.
+&lt;\MATTPics\CancelDivision_Example2.PNG&gt;
+You can also apply this technique to variable denominators.
+&lt;\MATTPics\CancelDivision_Example.PNG&gt;
+If you cannot factor out any common terms, you can separate the fraction into several terms. This can only be done if the numerator is multiple terms.
+&lt;\MATTPics\CancelDivision_Separate.PNG&gt;
+If the numerator is only one term, the fraction can still be separated but only by a process called partial fraction decomposition.
+&lt;\MATTPics\PartialFractions.PNG&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Multiplying two polynomials involves multiplying each term in both of the polynomials. Remember that when an entire equation is raised to a power, you can't simply distribute the power, you have to multiply the equations together. This process is commonly referred to as FOIL. FOIL stands for
+First
+Outside
+Inside
+Last
+It represents the order of multiplying each term in the two equations. Here are a couple examples:
+&lt;\MATTPics\FOIL_BreakDown.png&gt;
+&lt;\MATTPics\FOIL_Example.png&gt;
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Order of Operations (PEDMAS)
+There is a hierarchy of operations when evaluating mathematical expressions:
+1. Parentheses: Always evaluate expressions inside parentheses first.
+2. Exponents: Next apply any exponents in the expression (This step also applies to radicals).
+3/4. Division/Multiplication: Since division and multiplication are the same step, evaluate from right to left.
+5/6. Addition/Subtraction: Also evaluate addition and subtraction from right to left.
+A way to help remember this order is to use the pneumonic device Please Excuse My Dear Aunt Sally.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A number with an exponent written above it is a shorter way to write how many times a number is multiplied by itself.
+The larger number is the base and the smaller number written above it is the exponent.
+&lt;\MATTPics\SimpleExponent_BaseExp.png&gt;
+The base is multiplied by itself the number of times that the exponent indicates:
+&lt;\MATTPics\SimpleExponent_Expanded.png&gt;
+This is also called raising a number to a power.
+A negative exponent will be positive in the denominator of an expression. Once the exponent is positive, it can be evaluated normally.
+&lt;\MATTPics\SimpleExponent_Negative.png&gt;
 </t>
   </si>
 </sst>
@@ -782,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B42"/>
+  <dimension ref="A1:B63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -807,7 +1016,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="72" x14ac:dyDescent="0.3">
@@ -815,23 +1024,23 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
@@ -839,15 +1048,15 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
@@ -855,279 +1064,447 @@
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>124</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
+        <v>123</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="388.8" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>37</v>
+        <v>122</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>40</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>42</v>
+        <v>120</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>49</v>
+        <v>119</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>69</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="230.4" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="259.2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>75</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="216" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>79</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="201.6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>80</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="72" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B46" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="2" t="s">
+    </row>
+    <row r="47" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B48" s="2" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A50" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="72" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A58" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A59" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A60" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A61" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A62" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A63" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>